<commit_message>
fixed example tables bug
</commit_message>
<xml_diff>
--- a/data/picogreen1.xlsx
+++ b/data/picogreen1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyoungblut/ownCloud/Ley_lab/dev/R/shiny/plate_reader/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="27800" windowHeight="14640"/>
   </bookViews>
@@ -16,20 +11,20 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="153">
   <si>
     <t>Well ID</t>
   </si>
@@ -55,12 +50,6 @@
     <t>CV (%)</t>
   </si>
   <si>
-    <t>BLK</t>
-  </si>
-  <si>
-    <t>Sample blank</t>
-  </si>
-  <si>
     <t>H1</t>
   </si>
   <si>
@@ -436,33 +425,18 @@
     <t>A1</t>
   </si>
   <si>
-    <t>*90024*</t>
-  </si>
-  <si>
-    <t>?????</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
-    <t>*87916*</t>
-  </si>
-  <si>
     <t>STD2</t>
   </si>
   <si>
     <t>B1</t>
   </si>
   <si>
-    <t>*80911*</t>
-  </si>
-  <si>
     <t>B2</t>
   </si>
   <si>
-    <t>*79528*</t>
-  </si>
-  <si>
     <t>STD3</t>
   </si>
   <si>
@@ -506,6 +480,9 @@
   </si>
   <si>
     <t>G2</t>
+  </si>
+  <si>
+    <t>STD8</t>
   </si>
 </sst>
 </file>
@@ -642,7 +619,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -677,7 +654,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -888,11 +865,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,1964 +900,2128 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>100</v>
+      </c>
       <c r="E2" s="3">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="F2" s="3">
         <v>2</v>
       </c>
       <c r="G2" s="3">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="H2" s="3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3">
-        <v>4.7140000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>9.6310000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>100</v>
+      </c>
       <c r="E3" s="3">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
       <c r="E4" s="3">
-        <v>50776</v>
+        <v>1369</v>
       </c>
       <c r="F4" s="3">
         <v>2</v>
       </c>
       <c r="G4" s="3">
-        <v>50866</v>
+        <v>1370</v>
       </c>
       <c r="H4" s="3">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
       <c r="E5" s="3">
-        <v>50956</v>
+        <v>1371</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>100</v>
+      </c>
       <c r="E6" s="3">
-        <v>47156</v>
+        <v>2952</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>47825</v>
+        <v>2932</v>
       </c>
       <c r="H6" s="3">
-        <v>945</v>
+        <v>28</v>
       </c>
       <c r="I6" s="3">
-        <v>1.9770000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.96499999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D7" s="3">
+        <v>100</v>
+      </c>
       <c r="E7" s="3">
-        <v>48493</v>
+        <v>2912</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="3">
+        <v>100</v>
+      </c>
       <c r="E8" s="3">
-        <v>58353</v>
+        <v>7517</v>
       </c>
       <c r="F8" s="3">
         <v>2</v>
       </c>
       <c r="G8" s="3">
-        <v>57726</v>
+        <v>7493</v>
       </c>
       <c r="H8" s="3">
-        <v>887</v>
+        <v>35</v>
       </c>
       <c r="I8" s="3">
-        <v>1.5369999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="D9" s="3">
+        <v>100</v>
+      </c>
       <c r="E9" s="3">
-        <v>57098</v>
+        <v>7468</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="D10" s="3">
+        <v>100</v>
+      </c>
       <c r="E10" s="3">
-        <v>68109</v>
+        <v>9980</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
       </c>
       <c r="G10" s="3">
-        <v>65583</v>
+        <v>10070</v>
       </c>
       <c r="H10" s="3">
-        <v>3573</v>
+        <v>127</v>
       </c>
       <c r="I10" s="3">
-        <v>5.4480000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.2569999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D11" s="3">
+        <v>100</v>
+      </c>
       <c r="E11" s="3">
-        <v>63056</v>
+        <v>10159</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D12" s="3">
+        <v>100</v>
+      </c>
       <c r="E12" s="3">
-        <v>69511</v>
+        <v>4695</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>68349</v>
+        <v>4706</v>
       </c>
       <c r="H12" s="3">
-        <v>1643</v>
+        <v>16</v>
       </c>
       <c r="I12" s="3">
-        <v>2.4039999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="D13" s="3">
+        <v>100</v>
+      </c>
       <c r="E13" s="3">
-        <v>67187</v>
+        <v>4717</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="D14" s="3">
+        <v>100</v>
+      </c>
       <c r="E14" s="3">
-        <v>3094</v>
+        <v>1734</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
       </c>
       <c r="G14" s="3">
-        <v>3184</v>
+        <v>1772</v>
       </c>
       <c r="H14" s="3">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="I14" s="3">
-        <v>3.9969999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.9940000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D15" s="3">
+        <v>100</v>
+      </c>
       <c r="E15" s="3">
-        <v>3274</v>
+        <v>1809</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D16" s="3">
+        <v>100</v>
+      </c>
       <c r="E16" s="3">
-        <v>29</v>
+        <v>10335</v>
       </c>
       <c r="F16" s="3">
         <v>2</v>
       </c>
       <c r="G16" s="3">
-        <v>33</v>
+        <v>10504</v>
       </c>
       <c r="H16" s="3">
-        <v>5</v>
+        <v>239</v>
       </c>
       <c r="I16" s="3">
-        <v>15.23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.2749999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="D17" s="3">
+        <v>100</v>
+      </c>
       <c r="E17" s="3">
-        <v>36</v>
+        <v>10673</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D18" s="3">
+        <v>100</v>
+      </c>
       <c r="E18" s="3">
-        <v>32</v>
+        <v>5501</v>
       </c>
       <c r="F18" s="3">
         <v>2</v>
       </c>
       <c r="G18" s="3">
-        <v>31</v>
+        <v>5515</v>
       </c>
       <c r="H18" s="3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="I18" s="3">
-        <v>6.9550000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="D19" s="3">
+        <v>100</v>
+      </c>
       <c r="E19" s="3">
-        <v>29</v>
+        <v>5529</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="D20" s="3">
+        <v>100</v>
+      </c>
       <c r="E20" s="3">
-        <v>24</v>
+        <v>891</v>
       </c>
       <c r="F20" s="3">
         <v>2</v>
       </c>
       <c r="G20" s="3">
-        <v>29</v>
+        <v>868</v>
       </c>
       <c r="H20" s="3">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="I20" s="3">
-        <v>22.33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.7469999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D21" s="3">
+        <v>100</v>
+      </c>
       <c r="E21" s="3">
-        <v>33</v>
+        <v>845</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D22" s="3">
+        <v>100</v>
+      </c>
       <c r="E22" s="3">
-        <v>31</v>
+        <v>7359</v>
       </c>
       <c r="F22" s="3">
         <v>2</v>
       </c>
       <c r="G22" s="3">
-        <v>30</v>
+        <v>7272</v>
       </c>
       <c r="H22" s="3">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="I22" s="3">
-        <v>7.1909999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.6919999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D23" s="3">
+        <v>100</v>
+      </c>
       <c r="E23" s="3">
-        <v>28</v>
+        <v>7185</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="D24" s="3">
+        <v>100</v>
+      </c>
       <c r="E24" s="3">
-        <v>38</v>
+        <v>18880</v>
       </c>
       <c r="F24" s="3">
         <v>2</v>
       </c>
       <c r="G24" s="3">
-        <v>34</v>
+        <v>18645</v>
       </c>
       <c r="H24" s="3">
-        <v>6</v>
+        <v>333</v>
       </c>
       <c r="I24" s="3">
-        <v>18.997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.786</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="D25" s="3">
+        <v>100</v>
+      </c>
       <c r="E25" s="3">
-        <v>29</v>
+        <v>18409</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D26" s="3">
+        <v>100</v>
+      </c>
       <c r="E26" s="3">
-        <v>37</v>
+        <v>16812</v>
       </c>
       <c r="F26" s="3">
         <v>2</v>
       </c>
       <c r="G26" s="3">
-        <v>29</v>
+        <v>16501</v>
       </c>
       <c r="H26" s="3">
-        <v>11</v>
+        <v>440</v>
       </c>
       <c r="I26" s="3">
-        <v>39.012999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="D27" s="3">
+        <v>100</v>
+      </c>
       <c r="E27" s="3">
-        <v>21</v>
+        <v>16190</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="D28" s="3">
+        <v>100</v>
+      </c>
       <c r="E28" s="3">
-        <v>31</v>
+        <v>9862</v>
       </c>
       <c r="F28" s="3">
         <v>2</v>
       </c>
       <c r="G28" s="3">
-        <v>35</v>
+        <v>9542</v>
       </c>
       <c r="H28" s="3">
-        <v>5</v>
+        <v>453</v>
       </c>
       <c r="I28" s="3">
-        <v>14.347</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="D29" s="3">
+        <v>100</v>
+      </c>
       <c r="E29" s="3">
-        <v>38</v>
+        <v>9221</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="D30" s="3">
+        <v>100</v>
+      </c>
       <c r="E30" s="3">
-        <v>31</v>
+        <v>8273</v>
       </c>
       <c r="F30" s="3">
         <v>2</v>
       </c>
       <c r="G30" s="3">
-        <v>29</v>
+        <v>7936</v>
       </c>
       <c r="H30" s="3">
-        <v>4</v>
+        <v>477</v>
       </c>
       <c r="I30" s="3">
-        <v>12.404999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.0149999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D31" s="3">
+        <v>100</v>
+      </c>
       <c r="E31" s="3">
-        <v>26</v>
+        <v>7598</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D32" s="3">
+        <v>100</v>
+      </c>
       <c r="E32" s="3">
-        <v>26</v>
+        <v>1956</v>
       </c>
       <c r="F32" s="3">
         <v>2</v>
       </c>
       <c r="G32" s="3">
-        <v>29</v>
+        <v>1894</v>
       </c>
       <c r="H32" s="3">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="I32" s="3">
-        <v>14.63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.6680000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="D33" s="3">
+        <v>100</v>
+      </c>
       <c r="E33" s="3">
-        <v>32</v>
+        <v>1831</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="D34" s="3">
+        <v>100</v>
+      </c>
       <c r="E34" s="3">
-        <v>28</v>
+        <v>1293</v>
       </c>
       <c r="F34" s="3">
         <v>2</v>
       </c>
       <c r="G34" s="3">
-        <v>32</v>
+        <v>1300</v>
       </c>
       <c r="H34" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I34" s="3">
-        <v>15.712999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="D35" s="3">
+        <v>100</v>
+      </c>
       <c r="E35" s="3">
-        <v>35</v>
+        <v>1307</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D36" s="3">
+        <v>100</v>
+      </c>
       <c r="E36" s="3">
-        <v>27</v>
+        <v>1150</v>
       </c>
       <c r="F36" s="3">
         <v>2</v>
       </c>
       <c r="G36" s="3">
-        <v>28</v>
+        <v>1158</v>
       </c>
       <c r="H36" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I36" s="3">
-        <v>5.0510000000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="D37" s="3">
+        <v>100</v>
+      </c>
       <c r="E37" s="3">
-        <v>29</v>
+        <v>1165</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="D38" s="3">
+        <v>100</v>
+      </c>
       <c r="E38" s="3">
-        <v>27</v>
+        <v>1043</v>
       </c>
       <c r="F38" s="3">
         <v>2</v>
       </c>
       <c r="G38" s="3">
-        <v>30</v>
+        <v>1071</v>
       </c>
       <c r="H38" s="3">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="I38" s="3">
-        <v>11.984999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.633</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D39" s="3">
+        <v>100</v>
+      </c>
       <c r="E39" s="3">
-        <v>32</v>
+        <v>1098</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="D40" s="3">
+        <v>100</v>
+      </c>
       <c r="E40" s="3">
-        <v>29</v>
+        <v>2054</v>
       </c>
       <c r="F40" s="3">
         <v>2</v>
       </c>
       <c r="G40" s="3">
-        <v>31</v>
+        <v>2079</v>
       </c>
       <c r="H40" s="3">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="I40" s="3">
-        <v>9.1240000000000006</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.7010000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="D41" s="3">
+        <v>100</v>
+      </c>
       <c r="E41" s="3">
-        <v>33</v>
+        <v>2104</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="D42" s="3">
+        <v>100</v>
+      </c>
       <c r="E42" s="3">
-        <v>31</v>
+        <v>4857</v>
       </c>
       <c r="F42" s="3">
         <v>2</v>
       </c>
       <c r="G42" s="3">
-        <v>32</v>
+        <v>4853</v>
       </c>
       <c r="H42" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I42" s="3">
-        <v>4.4189999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D43" s="3">
+        <v>100</v>
+      </c>
       <c r="E43" s="3">
-        <v>33</v>
+        <v>4849</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="D44" s="3">
+        <v>100</v>
+      </c>
       <c r="E44" s="3">
-        <v>41</v>
+        <v>302</v>
       </c>
       <c r="F44" s="3">
         <v>2</v>
       </c>
       <c r="G44" s="3">
-        <v>36</v>
+        <v>278</v>
       </c>
       <c r="H44" s="3">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="I44" s="3">
-        <v>19.641999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12.486000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="D45" s="3">
+        <v>100</v>
+      </c>
       <c r="E45" s="3">
-        <v>31</v>
+        <v>253</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D46" s="3">
+        <v>100</v>
+      </c>
       <c r="E46" s="3">
-        <v>34</v>
+        <v>1560</v>
       </c>
       <c r="F46" s="3">
         <v>2</v>
       </c>
       <c r="G46" s="3">
-        <v>32</v>
+        <v>1590</v>
       </c>
       <c r="H46" s="3">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="I46" s="3">
-        <v>8.8390000000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="D47" s="3">
+        <v>100</v>
+      </c>
       <c r="E47" s="3">
-        <v>30</v>
+        <v>1619</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="D48" s="3">
+        <v>100</v>
+      </c>
       <c r="E48" s="3">
-        <v>33</v>
+        <v>2083</v>
       </c>
       <c r="F48" s="3">
         <v>2</v>
       </c>
       <c r="G48" s="3">
-        <v>36</v>
+        <v>2100</v>
       </c>
       <c r="H48" s="3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="I48" s="3">
-        <v>11.785</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="D49" s="3">
+        <v>100</v>
+      </c>
       <c r="E49" s="3">
-        <v>39</v>
+        <v>2117</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="D50" s="3">
+        <v>100</v>
+      </c>
       <c r="E50" s="3">
-        <v>27</v>
+        <v>880</v>
       </c>
       <c r="F50" s="3">
         <v>2</v>
       </c>
       <c r="G50" s="3">
-        <v>31</v>
+        <v>895</v>
       </c>
       <c r="H50" s="3">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="I50" s="3">
-        <v>16.228999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="D51" s="3">
+        <v>100</v>
+      </c>
       <c r="E51" s="3">
-        <v>34</v>
+        <v>910</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="D52" s="3">
+        <v>100</v>
+      </c>
       <c r="E52" s="3">
-        <v>35</v>
+        <v>4992</v>
       </c>
       <c r="F52" s="3">
         <v>2</v>
       </c>
       <c r="G52" s="3">
-        <v>35</v>
+        <v>4991</v>
       </c>
       <c r="H52" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D53" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="D53" s="3">
+        <v>100</v>
+      </c>
       <c r="E53" s="3">
-        <v>35</v>
+        <v>4990</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="D54" s="3">
+        <v>100</v>
+      </c>
       <c r="E54" s="3">
-        <v>30</v>
+        <v>9835</v>
       </c>
       <c r="F54" s="3">
         <v>2</v>
       </c>
       <c r="G54" s="3">
-        <v>31</v>
+        <v>9668</v>
       </c>
       <c r="H54" s="3">
-        <v>1</v>
+        <v>236</v>
       </c>
       <c r="I54" s="3">
-        <v>2.3180000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.4430000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="D55" s="3">
+        <v>100</v>
+      </c>
       <c r="E55" s="3">
-        <v>31</v>
+        <v>9501</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="D56" s="3">
+        <v>100</v>
+      </c>
       <c r="E56" s="3">
-        <v>31</v>
+        <v>1440</v>
       </c>
       <c r="F56" s="3">
         <v>2</v>
       </c>
       <c r="G56" s="3">
-        <v>28</v>
+        <v>1435</v>
       </c>
       <c r="H56" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I56" s="3">
-        <v>17.998999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D57" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D57" s="3">
+        <v>100</v>
+      </c>
       <c r="E57" s="3">
-        <v>24</v>
+        <v>1430</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="D58" s="3">
+        <v>100</v>
+      </c>
       <c r="E58" s="3">
-        <v>35</v>
+        <v>1036</v>
       </c>
       <c r="F58" s="3">
         <v>2</v>
       </c>
       <c r="G58" s="3">
-        <v>35</v>
+        <v>1072</v>
       </c>
       <c r="H58" s="3">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="I58" s="3">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.7489999999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="D59" s="3">
+        <v>100</v>
+      </c>
       <c r="E59" s="3">
-        <v>34</v>
+        <v>1108</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9">
       <c r="A60" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D60" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="D60" s="3">
+        <v>100</v>
+      </c>
       <c r="E60" s="3">
-        <v>38</v>
+        <v>4749</v>
       </c>
       <c r="F60" s="3">
         <v>2</v>
       </c>
       <c r="G60" s="3">
-        <v>33</v>
+        <v>4753</v>
       </c>
       <c r="H60" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I60" s="3">
-        <v>23.933</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="D61" s="3">
+        <v>100</v>
+      </c>
       <c r="E61" s="3">
-        <v>27</v>
+        <v>4756</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9">
       <c r="A62" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="D62" s="3">
+        <v>100</v>
+      </c>
       <c r="E62" s="3">
-        <v>33</v>
+        <v>15310</v>
       </c>
       <c r="F62" s="3">
         <v>2</v>
       </c>
       <c r="G62" s="3">
-        <v>33</v>
+        <v>14652</v>
       </c>
       <c r="H62" s="3">
-        <v>1</v>
+        <v>931</v>
       </c>
       <c r="I62" s="3">
-        <v>2.1760000000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.351</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D63" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="D63" s="3">
+        <v>100</v>
+      </c>
       <c r="E63" s="3">
-        <v>32</v>
+        <v>13994</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9">
       <c r="A64" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="D64" s="3">
+        <v>100</v>
+      </c>
       <c r="E64" s="3">
-        <v>29</v>
+        <v>1425</v>
       </c>
       <c r="F64" s="3">
         <v>2</v>
       </c>
       <c r="G64" s="3">
-        <v>30</v>
+        <v>1439</v>
       </c>
       <c r="H64" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I64" s="3">
-        <v>2.3969999999999998</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.3759999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D65" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="D65" s="3">
+        <v>100</v>
+      </c>
       <c r="E65" s="3">
-        <v>30</v>
+        <v>1453</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9">
       <c r="A66" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D66" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="D66" s="3">
+        <v>100</v>
+      </c>
       <c r="E66" s="3">
-        <v>24</v>
+        <v>854</v>
       </c>
       <c r="F66" s="3">
         <v>2</v>
       </c>
       <c r="G66" s="3">
-        <v>25</v>
+        <v>851</v>
       </c>
       <c r="H66" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I66" s="3">
-        <v>5.657</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="D67" s="3">
+        <v>100</v>
+      </c>
       <c r="E67" s="3">
-        <v>26</v>
+        <v>847</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9">
       <c r="A68" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D68" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="D68" s="3">
+        <v>100</v>
+      </c>
       <c r="E68" s="3">
-        <v>36</v>
+        <v>29976</v>
       </c>
       <c r="F68" s="3">
         <v>2</v>
       </c>
       <c r="G68" s="3">
-        <v>35</v>
+        <v>29862</v>
       </c>
       <c r="H68" s="3">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="I68" s="3">
-        <v>6.149</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D69" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="D69" s="3">
+        <v>100</v>
+      </c>
       <c r="E69" s="3">
-        <v>33</v>
+        <v>29748</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9">
       <c r="A70" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="D70" s="3">
+        <v>100</v>
+      </c>
       <c r="E70" s="3">
-        <v>24</v>
+        <v>1421</v>
       </c>
       <c r="F70" s="3">
         <v>2</v>
       </c>
       <c r="G70" s="3">
-        <v>26</v>
+        <v>1420</v>
       </c>
       <c r="H70" s="3">
         <v>2</v>
       </c>
       <c r="I70" s="3">
-        <v>8.3190000000000008</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D71" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="D71" s="3">
+        <v>100</v>
+      </c>
       <c r="E71" s="3">
-        <v>27</v>
+        <v>1418</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9">
       <c r="A72" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D72" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="D72" s="3">
+        <v>100</v>
+      </c>
       <c r="E72" s="3">
-        <v>29</v>
+        <v>4166</v>
       </c>
       <c r="F72" s="3">
         <v>2</v>
       </c>
       <c r="G72" s="3">
-        <v>28</v>
+        <v>3896</v>
       </c>
       <c r="H72" s="3">
-        <v>2</v>
+        <v>383</v>
       </c>
       <c r="I72" s="3">
-        <v>7.7140000000000004</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D73" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="D73" s="3">
+        <v>100</v>
+      </c>
       <c r="E73" s="3">
-        <v>26</v>
+        <v>3625</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9">
       <c r="A74" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D74" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="D74" s="3">
+        <v>100</v>
+      </c>
       <c r="E74" s="3">
-        <v>32</v>
+        <v>674</v>
       </c>
       <c r="F74" s="3">
         <v>2</v>
       </c>
       <c r="G74" s="3">
-        <v>32</v>
+        <v>891</v>
       </c>
       <c r="H74" s="3">
-        <v>1</v>
+        <v>307</v>
       </c>
       <c r="I74" s="3">
-        <v>2.2450000000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+        <v>34.442999999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D75" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="D75" s="3">
+        <v>100</v>
+      </c>
       <c r="E75" s="3">
-        <v>31</v>
+        <v>1108</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9">
       <c r="A76" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="D76" s="3">
+        <v>100</v>
+      </c>
       <c r="E76" s="3">
-        <v>33</v>
+        <v>12129</v>
       </c>
       <c r="F76" s="3">
         <v>2</v>
       </c>
       <c r="G76" s="3">
-        <v>33</v>
+        <v>10998</v>
       </c>
       <c r="H76" s="3">
-        <v>1</v>
+        <v>1599</v>
       </c>
       <c r="I76" s="3">
-        <v>2.1760000000000002</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+        <v>14.542999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D77" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="D77" s="3">
+        <v>100</v>
+      </c>
       <c r="E77" s="3">
-        <v>32</v>
+        <v>9867</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9">
       <c r="A78" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D78" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="D78" s="3">
+        <v>100</v>
+      </c>
       <c r="E78" s="3">
-        <v>27</v>
+        <v>20638</v>
       </c>
       <c r="F78" s="3">
         <v>2</v>
       </c>
       <c r="G78" s="3">
-        <v>26</v>
+        <v>19560</v>
       </c>
       <c r="H78" s="3">
-        <v>2</v>
+        <v>1525</v>
       </c>
       <c r="I78" s="3">
-        <v>8.3190000000000008</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.7939999999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D79" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="D79" s="3">
+        <v>100</v>
+      </c>
       <c r="E79" s="3">
-        <v>24</v>
+        <v>18482</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9">
       <c r="A80" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="D80" s="3">
+        <v>100</v>
+      </c>
       <c r="E80" s="3">
-        <v>33</v>
+        <v>29944</v>
       </c>
       <c r="F80" s="3">
         <v>2</v>
       </c>
       <c r="G80" s="3">
-        <v>32</v>
+        <v>28548</v>
       </c>
       <c r="H80" s="3">
-        <v>2</v>
+        <v>1974</v>
       </c>
       <c r="I80" s="3">
-        <v>6.734</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.9160000000000004</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="D81" s="3">
+        <v>100</v>
+      </c>
       <c r="E81" s="3">
-        <v>30</v>
+        <v>27152</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="24">
       <c r="A82" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B82" s="3"/>
+        <v>130</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="C82" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="D82" s="3">
+        <v>100</v>
+      </c>
       <c r="E82" s="3">
-        <v>22</v>
+        <v>283500</v>
       </c>
       <c r="F82" s="3">
         <v>2</v>
       </c>
       <c r="G82" s="3">
-        <v>26</v>
+        <v>282903</v>
       </c>
       <c r="H82" s="3">
-        <v>6</v>
+        <v>844</v>
       </c>
       <c r="I82" s="3">
-        <v>21.757000000000001</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D83" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="D83" s="3">
+        <v>100</v>
+      </c>
       <c r="E83" s="3">
-        <v>30</v>
+        <v>282306</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
     </row>
-    <row r="84" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="24">
       <c r="A84" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D84" s="3">
-        <v>75</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>135</v>
+        <v>80</v>
+      </c>
+      <c r="E84" s="3">
+        <v>227580</v>
       </c>
       <c r="F84" s="3">
-        <v>0</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G84" s="3">
+        <v>227777</v>
+      </c>
+      <c r="H84" s="3">
+        <v>278</v>
+      </c>
+      <c r="I84" s="3">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D85" s="3">
-        <v>75</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>138</v>
+        <v>80</v>
+      </c>
+      <c r="E85" s="3">
+        <v>227973</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
     </row>
-    <row r="86" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="24">
       <c r="A86" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D86" s="3">
-        <v>50</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>141</v>
+        <v>60</v>
+      </c>
+      <c r="E86" s="3">
+        <v>157143</v>
       </c>
       <c r="F86" s="3">
-        <v>0</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="G86" s="3">
+        <v>163894</v>
+      </c>
+      <c r="H86" s="3">
+        <v>9547</v>
+      </c>
+      <c r="I86" s="3">
+        <v>5.8250000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D87" s="3">
-        <v>50</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>143</v>
+        <v>60</v>
+      </c>
+      <c r="E87" s="3">
+        <v>170644</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
     </row>
-    <row r="88" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="24">
       <c r="A88" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D88" s="3">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E88" s="3">
-        <v>48087</v>
+        <v>106375</v>
       </c>
       <c r="F88" s="3">
         <v>2</v>
       </c>
       <c r="G88" s="3">
-        <v>47391</v>
+        <v>106076</v>
       </c>
       <c r="H88" s="3">
-        <v>984</v>
+        <v>424</v>
       </c>
       <c r="I88" s="3">
-        <v>2.077</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D89" s="3">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E89" s="3">
-        <v>46695</v>
+        <v>105776</v>
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
     </row>
-    <row r="90" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="24">
       <c r="A90" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D90" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E90" s="3">
-        <v>19984</v>
+        <v>52875</v>
       </c>
       <c r="F90" s="3">
         <v>2</v>
       </c>
       <c r="G90" s="3">
-        <v>20151</v>
+        <v>52817</v>
       </c>
       <c r="H90" s="3">
-        <v>236</v>
+        <v>82</v>
       </c>
       <c r="I90" s="3">
-        <v>1.1719999999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D91" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E91" s="3">
-        <v>20318</v>
+        <v>52759</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
     </row>
-    <row r="92" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="24">
       <c r="A92" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D92" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E92" s="3">
-        <v>10288</v>
+        <v>27170</v>
       </c>
       <c r="F92" s="3">
         <v>2</v>
       </c>
       <c r="G92" s="3">
-        <v>10048</v>
+        <v>27174</v>
       </c>
       <c r="H92" s="3">
-        <v>339</v>
+        <v>6</v>
       </c>
       <c r="I92" s="3">
-        <v>3.3780000000000001</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D93" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E93" s="3">
-        <v>9808</v>
+        <v>27178</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
     </row>
-    <row r="94" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="24">
       <c r="A94" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D94" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E94" s="3">
-        <v>3962</v>
+        <v>12987</v>
       </c>
       <c r="F94" s="3">
         <v>2</v>
       </c>
       <c r="G94" s="3">
-        <v>3898</v>
+        <v>12969</v>
       </c>
       <c r="H94" s="3">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="I94" s="3">
-        <v>2.34</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D95" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E95" s="3">
-        <v>3833</v>
+        <v>12950</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
     </row>
-    <row r="96" spans="1:9" ht="26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="24">
       <c r="A96" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="D96" s="3">
         <v>0</v>
       </c>
       <c r="E96" s="3">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F96" s="3">
         <v>2</v>
       </c>
       <c r="G96" s="3">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="H96" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I96" s="3">
-        <v>10.879</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.992</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="D97" s="3">
         <v>0</v>
       </c>
       <c r="E97" s="3">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -2887,7 +3030,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2897,9 +3045,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2909,8 +3062,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>